<commit_message>
preview feature upload bug fixed
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="85">
   <si>
     <t>Language_id</t>
   </si>
@@ -28,13 +28,37 @@
     <t>Updated_date</t>
   </si>
   <si>
-    <t/>
+    <t>US-en</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:26:48.000Z</t>
+  </si>
+  <si>
+    <t>IN-kn</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:26:50.000Z</t>
+  </si>
+  <si>
+    <t>IN-hi</t>
   </si>
   <si>
     <t>Page_id</t>
   </si>
   <si>
     <t>Page_name</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Signup</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:26:51.000Z</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
   </si>
   <si>
     <t>Label_id</t>
@@ -46,7 +70,205 @@
     <t>Label_value</t>
   </si>
   <si>
+    <t>userDatabase</t>
+  </si>
+  <si>
+    <t>User Database</t>
+  </si>
+  <si>
+    <t>ಯೂಸರ್ ಡೇಟಾಬೇಸ್</t>
+  </si>
+  <si>
+    <t>यूजर डेटाबेस</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:26:52.000Z</t>
+  </si>
+  <si>
+    <t>signUp</t>
+  </si>
+  <si>
+    <t>Sign Up</t>
+  </si>
+  <si>
+    <t>ಸೈನ್ ಅಪ್</t>
+  </si>
+  <si>
+    <t>सैन अप</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>ಯೂಸರ್ ನೇಮ್</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:26:53.000Z</t>
+  </si>
+  <si>
+    <t>यूजर नाम</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>ಪಾಸ್ವರ್ಡ್</t>
+  </si>
+  <si>
+    <t>पासवर्ड</t>
+  </si>
+  <si>
+    <t>signIn</t>
+  </si>
+  <si>
+    <t>Sign In</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:26:54.000Z</t>
+  </si>
+  <si>
+    <t>ಸೈನ್ ಇನ್</t>
+  </si>
+  <si>
+    <t>सैन इन</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>ಲಾಗಿನ್</t>
+  </si>
+  <si>
+    <t>लॉगिन</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:26:55.000Z</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>ಫಸ್ಟ್ ನೇಮ್</t>
+  </si>
+  <si>
+    <t>फर्स्ट नाम</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>ಲಾಸ್ಟ ನೇಮ್</t>
+  </si>
+  <si>
+    <t>लास्ट नाम</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:26:56.000Z</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>ಇಮೇಲ್</t>
+  </si>
+  <si>
+    <t>ईमेल</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>ಲಾಗ್ಔಟ್</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:26:57.000Z</t>
+  </si>
+  <si>
+    <t>लॉगआउट</t>
+  </si>
+  <si>
+    <t>welcome</t>
+  </si>
+  <si>
+    <t>Welcome User</t>
+  </si>
+  <si>
+    <t>ಸ್ವಾಗತ ಯೂಸರ್</t>
+  </si>
+  <si>
+    <t>स्वागत यूजर</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ಐಡೀ</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:26:58.000Z</t>
+  </si>
+  <si>
+    <t>आईडी</t>
+  </si>
+  <si>
     <t>Page_map_id</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:26:59.000Z</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:27:00.000Z</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:27:01.000Z</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:27:02.000Z</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:27:03.000Z</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:27:04.000Z</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:27:05.000Z</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:27:06.000Z</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:27:07.000Z</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:27:08.000Z</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:27:09.000Z</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:27:10.000Z</t>
+  </si>
+  <si>
+    <t>2022-03-30T04:27:11.000Z</t>
   </si>
 </sst>
 </file>
@@ -359,45 +581,45 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
+      <c r="A2" s="2">
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
+      <c r="A3" s="2">
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
+      <c r="A4" s="2">
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1418,10 +1640,10 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1431,45 +1653,45 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
+      <c r="A2" s="2">
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
+      <c r="A3" s="2">
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
+      <c r="A4" s="2">
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2491,13 +2713,13 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -2510,723 +2732,723 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="B5" s="5" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>4</v>
+        <v>24</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
+      <c r="A6" s="4">
+        <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>4</v>
+        <v>25</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
+      <c r="A7" s="4">
+        <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
+      <c r="A8" s="4">
+        <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>4</v>
+        <v>28</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>4</v>
+      <c r="A9" s="4">
+        <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>4</v>
+        <v>29</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>4</v>
+      <c r="A10" s="4">
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>4</v>
+        <v>31</v>
+      </c>
+      <c r="D10" s="4">
+        <v>3</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>4</v>
+      <c r="A11" s="4">
+        <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>4</v>
+        <v>32</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>4</v>
+      <c r="A12" s="4">
+        <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>4</v>
+        <v>33</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>4</v>
+      <c r="A13" s="4">
+        <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>4</v>
+        <v>34</v>
+      </c>
+      <c r="D13" s="4">
+        <v>3</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>4</v>
+      <c r="A14" s="4">
+        <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>4</v>
+        <v>36</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>4</v>
+      <c r="A15" s="4">
+        <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>4</v>
+        <v>38</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>4</v>
+      <c r="A16" s="4">
+        <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>4</v>
+        <v>39</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>4</v>
+      <c r="A17" s="4">
+        <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>4</v>
+      <c r="A18" s="4">
+        <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>4</v>
+      <c r="A19" s="4">
+        <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>4</v>
+        <v>42</v>
+      </c>
+      <c r="D19" s="4">
+        <v>3</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>4</v>
+      <c r="A20" s="4">
+        <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>4</v>
+        <v>45</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>4</v>
+      <c r="A21" s="4">
+        <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>4</v>
+        <v>46</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>4</v>
+      <c r="A22" s="4">
+        <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>4</v>
+        <v>47</v>
+      </c>
+      <c r="D22" s="4">
+        <v>3</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>4</v>
+      <c r="A23" s="4">
+        <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>4</v>
+        <v>49</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>4</v>
+      <c r="A24" s="4">
+        <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>4</v>
+        <v>50</v>
+      </c>
+      <c r="D24" s="4">
+        <v>2</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>4</v>
+      <c r="A25" s="4">
+        <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>4</v>
+        <v>51</v>
+      </c>
+      <c r="D25" s="4">
+        <v>3</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>4</v>
+      <c r="A26" s="4">
+        <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>4</v>
+        <v>54</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>4</v>
+      <c r="A27" s="4">
+        <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>4</v>
+        <v>55</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>4</v>
+      <c r="A28" s="4">
+        <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>4</v>
+        <v>56</v>
+      </c>
+      <c r="D28" s="4">
+        <v>3</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>4</v>
+      <c r="A29" s="4">
+        <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>4</v>
+        <v>58</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>4</v>
+      <c r="A30" s="4">
+        <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>4</v>
+        <v>59</v>
+      </c>
+      <c r="D30" s="4">
+        <v>2</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>4</v>
+      <c r="A31" s="4">
+        <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>4</v>
+        <v>61</v>
+      </c>
+      <c r="D31" s="4">
+        <v>3</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>4</v>
+      <c r="A32" s="4">
+        <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>4</v>
+        <v>63</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>4</v>
+      <c r="A33" s="4">
+        <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>4</v>
+        <v>64</v>
+      </c>
+      <c r="D33" s="4">
+        <v>2</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>4</v>
+      <c r="A34" s="4">
+        <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>4</v>
+        <v>65</v>
+      </c>
+      <c r="D34" s="4">
+        <v>3</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>4</v>
+      <c r="A35" s="4">
+        <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>4</v>
+        <v>67</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>4</v>
+      <c r="A36" s="4">
+        <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>4</v>
+        <v>68</v>
+      </c>
+      <c r="D36" s="4">
+        <v>2</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>4</v>
+      <c r="A37" s="4">
+        <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>4</v>
+        <v>70</v>
+      </c>
+      <c r="D37" s="4">
+        <v>3</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -6331,13 +6553,13 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -6347,1074 +6569,1074 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4">
+        <v>11</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4">
+        <v>13</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4">
+        <v>15</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4">
+        <v>16</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4">
+        <v>2</v>
+      </c>
+      <c r="C18" s="4">
+        <v>17</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
+        <v>2</v>
+      </c>
+      <c r="C19" s="4">
+        <v>18</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4">
+        <v>2</v>
+      </c>
+      <c r="C20" s="4">
+        <v>19</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4">
+        <v>2</v>
+      </c>
+      <c r="C21" s="4">
+        <v>20</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4">
+        <v>2</v>
+      </c>
+      <c r="C22" s="4">
+        <v>21</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4">
+        <v>2</v>
+      </c>
+      <c r="C23" s="4">
+        <v>22</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4">
+        <v>2</v>
+      </c>
+      <c r="C24" s="4">
+        <v>23</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4">
+        <v>24</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4">
+        <v>2</v>
+      </c>
+      <c r="C26" s="4">
+        <v>25</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4">
+        <v>2</v>
+      </c>
+      <c r="C27" s="4">
+        <v>26</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4">
+        <v>2</v>
+      </c>
+      <c r="C28" s="4">
+        <v>27</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4">
+        <v>3</v>
+      </c>
+      <c r="C29" s="4">
+        <v>28</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4">
+        <v>3</v>
+      </c>
+      <c r="C30" s="4">
+        <v>29</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4">
+        <v>3</v>
+      </c>
+      <c r="C31" s="4">
+        <v>30</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="4">
+        <v>3</v>
+      </c>
+      <c r="C32" s="4">
+        <v>31</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="4">
+        <v>3</v>
+      </c>
+      <c r="C33" s="4">
+        <v>32</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="4">
+        <v>3</v>
+      </c>
+      <c r="C34" s="4">
+        <v>33</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" s="4">
+        <v>3</v>
+      </c>
+      <c r="C35" s="4">
+        <v>34</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="4">
+        <v>3</v>
+      </c>
+      <c r="C36" s="4">
+        <v>35</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="4">
+        <v>3</v>
+      </c>
+      <c r="C37" s="4">
+        <v>36</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4">
+        <v>2</v>
+      </c>
+      <c r="C38" s="4">
+        <v>1</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" s="4">
+        <v>2</v>
+      </c>
+      <c r="C39" s="4">
+        <v>2</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4">
+        <v>2</v>
+      </c>
+      <c r="C40" s="4">
+        <v>3</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4">
+        <v>2</v>
+      </c>
+      <c r="C41" s="4">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="D41" s="3" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>4</v>
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4">
+        <v>2</v>
+      </c>
+      <c r="C42" s="4">
+        <v>5</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>4</v>
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" s="4">
+        <v>2</v>
+      </c>
+      <c r="C43" s="4">
+        <v>6</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>4</v>
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" s="4">
+        <v>2</v>
+      </c>
+      <c r="C44" s="4">
+        <v>7</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>4</v>
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" s="4">
+        <v>2</v>
+      </c>
+      <c r="C45" s="4">
+        <v>8</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>4</v>
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" s="4">
+        <v>2</v>
+      </c>
+      <c r="C46" s="4">
+        <v>9</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>4</v>
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" s="4">
+        <v>2</v>
+      </c>
+      <c r="C47" s="4">
+        <v>10</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>4</v>
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" s="4">
+        <v>2</v>
+      </c>
+      <c r="C48" s="4">
+        <v>11</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>4</v>
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" s="4">
+        <v>2</v>
+      </c>
+      <c r="C49" s="4">
+        <v>12</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>4</v>
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" s="4">
+        <v>3</v>
+      </c>
+      <c r="C50" s="4">
+        <v>7</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>4</v>
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" s="4">
+        <v>3</v>
+      </c>
+      <c r="C51" s="4">
+        <v>8</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>4</v>
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+      <c r="B52" s="4">
+        <v>3</v>
+      </c>
+      <c r="C52" s="4">
+        <v>9</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>4</v>
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+      <c r="B53" s="4">
+        <v>3</v>
+      </c>
+      <c r="C53" s="4">
+        <v>19</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>4</v>
+      <c r="A54" s="2">
+        <v>53</v>
+      </c>
+      <c r="B54" s="4">
+        <v>3</v>
+      </c>
+      <c r="C54" s="4">
+        <v>20</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>4</v>
+      <c r="A55" s="2">
+        <v>54</v>
+      </c>
+      <c r="B55" s="4">
+        <v>3</v>
+      </c>
+      <c r="C55" s="4">
+        <v>21</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>4</v>
+      <c r="A56" s="2">
+        <v>55</v>
+      </c>
+      <c r="B56" s="4">
+        <v>3</v>
+      </c>
+      <c r="C56" s="4">
+        <v>22</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>4</v>
+      <c r="A57" s="2">
+        <v>56</v>
+      </c>
+      <c r="B57" s="4">
+        <v>3</v>
+      </c>
+      <c r="C57" s="4">
+        <v>23</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>4</v>
+      <c r="A58" s="2">
+        <v>57</v>
+      </c>
+      <c r="B58" s="4">
+        <v>3</v>
+      </c>
+      <c r="C58" s="4">
+        <v>24</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>4</v>
+      <c r="A59" s="2">
+        <v>58</v>
+      </c>
+      <c r="B59" s="4">
+        <v>3</v>
+      </c>
+      <c r="C59" s="4">
+        <v>25</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>4</v>
+      <c r="A60" s="2">
+        <v>59</v>
+      </c>
+      <c r="B60" s="4">
+        <v>3</v>
+      </c>
+      <c r="C60" s="4">
+        <v>26</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>4</v>
+      <c r="A61" s="2">
+        <v>60</v>
+      </c>
+      <c r="B61" s="4">
+        <v>3</v>
+      </c>
+      <c r="C61" s="4">
+        <v>27</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>4</v>
+      <c r="A62" s="2">
+        <v>61</v>
+      </c>
+      <c r="B62" s="4">
+        <v>3</v>
+      </c>
+      <c r="C62" s="4">
+        <v>1</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>4</v>
+      <c r="A63" s="2">
+        <v>62</v>
+      </c>
+      <c r="B63" s="4">
+        <v>3</v>
+      </c>
+      <c r="C63" s="4">
+        <v>2</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>4</v>
+      <c r="A64" s="2">
+        <v>63</v>
+      </c>
+      <c r="B64" s="4">
+        <v>3</v>
+      </c>
+      <c r="C64" s="4">
+        <v>3</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>